<commit_message>
Some more todo items and BOM components
</commit_message>
<xml_diff>
--- a/bom/ProQ2-group1-BOM.xlsx
+++ b/bom/ProQ2-group1-BOM.xlsx
@@ -361,8 +361,8 @@
   </sheetPr>
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D61" activeCellId="0" sqref="D61"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -661,6 +661,9 @@
       <c r="B18" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="C18" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="F18" s="0" t="n">
         <f aca="false">C18 * E18</f>
         <v>0</v>
@@ -670,6 +673,9 @@
       <c r="B19" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="C19" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="F19" s="0" t="n">
         <f aca="false">C19 * E19</f>
         <v>0</v>
@@ -679,6 +685,9 @@
       <c r="B20" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="C20" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="F20" s="0" t="n">
         <f aca="false">C20 * E20</f>
         <v>0</v>
@@ -688,6 +697,9 @@
       <c r="B21" s="0" t="s">
         <v>25</v>
       </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="F21" s="0" t="n">
         <f aca="false">C21 * E21</f>
         <v>0</v>
@@ -697,6 +709,9 @@
       <c r="B22" s="0" t="s">
         <v>26</v>
       </c>
+      <c r="C22" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="F22" s="0" t="n">
         <f aca="false">C22 * E22</f>
         <v>0</v>
@@ -720,11 +735,13 @@
         <v>3.26</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="0" t="n">
@@ -732,11 +749,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="0" t="n">
@@ -744,11 +763,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="0" t="n">

</xml_diff>

<commit_message>
Bom fixed and dcu fixed
</commit_message>
<xml_diff>
--- a/bom/ProQ2-group1-BOM.xlsx
+++ b/bom/ProQ2-group1-BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -173,10 +173,7 @@
     <t>Digital control unit</t>
   </si>
   <si>
-    <t>ATMEGA328-PU</t>
-  </si>
-  <si>
-    <t>SUB_D connector</t>
+    <t>IC1: ATMEGA328-PU</t>
   </si>
   <si>
     <t>MCP4251-103E/P</t>
@@ -194,16 +191,13 @@
     <t>C1/C2: 22pF</t>
   </si>
   <si>
-    <t>D1/D2:LED (red)</t>
-  </si>
-  <si>
-    <t>D3:1N4148</t>
-  </si>
-  <si>
-    <t>R1/R2: 150</t>
-  </si>
-  <si>
-    <t>R3/R4: 200</t>
+    <t>LED1/LED2: red led</t>
+  </si>
+  <si>
+    <t>D1:1N4148</t>
+  </si>
+  <si>
+    <t>R1/R2/R3: 150</t>
   </si>
   <si>
     <t>VO617A-2</t>
@@ -325,7 +319,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -342,15 +336,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -360,10 +346,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -383,13 +365,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="A68" activeCellId="0" sqref="A68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.9676113360324"/>
     <col collapsed="false" hidden="false" max="5" min="2" style="0" width="9.1417004048583"/>
@@ -439,9 +421,7 @@
         <f aca="false">B3 * D3</f>
         <v>4.45</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="5"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -460,9 +440,7 @@
         <f aca="false">B4 * D4</f>
         <v>24.98</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="5"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -559,8 +537,8 @@
       <c r="B10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="4" t="n">
+      <c r="C10" s="3"/>
+      <c r="D10" s="0" t="n">
         <v>0.02</v>
       </c>
       <c r="E10" s="0" t="n">
@@ -575,7 +553,7 @@
       <c r="B11" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="7" t="n">
+      <c r="C11" s="5" t="n">
         <v>1102157</v>
       </c>
       <c r="D11" s="0" t="n">
@@ -587,13 +565,13 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="7" t="n">
+      <c r="C12" s="5" t="n">
         <v>2296025</v>
       </c>
       <c r="D12" s="0" t="n">
@@ -647,7 +625,7 @@
       <c r="B15" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C15" s="7" t="n">
+      <c r="C15" s="5" t="n">
         <v>1123175</v>
       </c>
       <c r="D15" s="0" t="n">
@@ -781,16 +759,16 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="8" t="n">
+      <c r="B24" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="C24" s="7" t="n">
+      <c r="C24" s="5" t="n">
         <v>2346523</v>
       </c>
-      <c r="D24" s="8" t="n">
+      <c r="D24" s="6" t="n">
         <v>1.63</v>
       </c>
       <c r="E24" s="0" t="n">
@@ -802,10 +780,10 @@
       <c r="A25" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="8" t="n">
+      <c r="B25" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="C25" s="7"/>
+      <c r="C25" s="5"/>
       <c r="D25" s="0" t="n">
         <v>0.1</v>
       </c>
@@ -818,10 +796,10 @@
       <c r="A26" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" s="7"/>
+      <c r="B26" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5"/>
       <c r="D26" s="0" t="n">
         <v>0.1</v>
       </c>
@@ -834,10 +812,10 @@
       <c r="A27" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" s="7"/>
+      <c r="B27" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5"/>
       <c r="D27" s="0" t="n">
         <v>0.1</v>
       </c>
@@ -850,8 +828,8 @@
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="7"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
@@ -878,7 +856,7 @@
       <c r="B30" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C30" s="7" t="n">
+      <c r="C30" s="5" t="n">
         <v>1106092</v>
       </c>
       <c r="D30" s="0" t="n">
@@ -1168,7 +1146,7 @@
       <c r="B48" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C48" s="7" t="n">
+      <c r="C48" s="5" t="n">
         <v>2445620</v>
       </c>
       <c r="D48" s="0" t="n">
@@ -1208,35 +1186,35 @@
         <v>53</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C51" s="3" t="n">
-        <v>1075277</v>
+        <v>1578442</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>1.79</v>
+        <v>0.921</v>
       </c>
       <c r="E51" s="0" t="n">
         <f aca="false">B51 * D51</f>
-        <v>1.79</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>3.684</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>54</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C52" s="3" t="n">
-        <v>1578442</v>
+        <v>1</v>
+      </c>
+      <c r="C52" s="5" t="n">
+        <v>2445626</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>0.921</v>
+        <v>0.44</v>
       </c>
       <c r="E52" s="0" t="n">
         <f aca="false">B52 * D52</f>
-        <v>3.684</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1244,17 +1222,17 @@
         <v>55</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C53" s="7" t="n">
-        <v>2445626</v>
+        <v>4</v>
+      </c>
+      <c r="C53" s="5" t="n">
+        <v>2445621</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>0.44</v>
+        <v>0.198</v>
       </c>
       <c r="E53" s="0" t="n">
         <f aca="false">B53 * D53</f>
-        <v>0.44</v>
+        <v>0.792</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1262,51 +1240,51 @@
         <v>56</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C54" s="7" t="n">
-        <v>2445621</v>
+        <v>1</v>
+      </c>
+      <c r="C54" s="5" t="n">
+        <v>1611761</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>0.198</v>
+        <v>0.378</v>
       </c>
       <c r="E54" s="0" t="n">
         <f aca="false">B54 * D54</f>
-        <v>0.792</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.378</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>57</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C55" s="7" t="n">
-        <v>1611761</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C55" s="3"/>
       <c r="D55" s="0" t="n">
-        <v>0.378</v>
+        <v>0.1</v>
       </c>
       <c r="E55" s="0" t="n">
         <f aca="false">B55 * D55</f>
-        <v>0.378</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C56" s="3"/>
+      <c r="C56" s="5" t="n">
+        <v>2112100</v>
+      </c>
       <c r="D56" s="0" t="n">
-        <v>0.1</v>
+        <v>0.214</v>
       </c>
       <c r="E56" s="0" t="n">
         <f aca="false">B56 * D56</f>
-        <v>0.2</v>
+        <v>0.428</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1314,85 +1292,85 @@
         <v>59</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C57" s="7" t="n">
-        <v>2112100</v>
+        <v>1</v>
+      </c>
+      <c r="C57" s="5" t="n">
+        <v>9565124</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>0.214</v>
+        <v>0.0203</v>
       </c>
       <c r="E57" s="0" t="n">
         <f aca="false">B57 * D57</f>
-        <v>0.428</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.0203</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>60</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C58" s="7" t="n">
-        <v>9565124</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C58" s="3"/>
       <c r="D58" s="0" t="n">
-        <v>0.0203</v>
+        <v>0.02</v>
       </c>
       <c r="E58" s="0" t="n">
         <f aca="false">B58 * D58</f>
-        <v>0.0203</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>61</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C59" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="C59" s="5" t="n">
+        <v>2251550</v>
+      </c>
       <c r="D59" s="0" t="n">
-        <v>0.02</v>
+        <v>0.187</v>
       </c>
       <c r="E59" s="0" t="n">
         <f aca="false">B59 * D59</f>
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.187</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>62</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C60" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="C60" s="5" t="n">
+        <v>1280804</v>
+      </c>
       <c r="D60" s="0" t="n">
-        <v>0.02</v>
+        <v>1.45</v>
       </c>
       <c r="E60" s="0" t="n">
         <f aca="false">B60 * D60</f>
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>63</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C61" s="7" t="n">
-        <v>2251550</v>
-      </c>
+      <c r="C61" s="3"/>
       <c r="D61" s="0" t="n">
-        <v>0.187</v>
+        <v>0.1</v>
       </c>
       <c r="E61" s="0" t="n">
         <f aca="false">B61 * D61</f>
-        <v>0.187</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1402,103 +1380,103 @@
       <c r="B62" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C62" s="7" t="n">
-        <v>1280804</v>
+      <c r="C62" s="5" t="n">
+        <v>2445619</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>1.45</v>
+        <v>0.204</v>
       </c>
       <c r="E62" s="0" t="n">
         <f aca="false">B62 * D62</f>
-        <v>1.45</v>
+        <v>0.204</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B63" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="C63" s="3"/>
-      <c r="D63" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E63" s="0" t="n">
-        <f aca="false">B63 * D63</f>
-        <v>0.1</v>
-      </c>
     </row>
     <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="6" t="s">
         <v>66</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C64" s="7" t="n">
-        <v>2445619</v>
+        <v>10</v>
+      </c>
+      <c r="C64" s="5" t="n">
+        <v>3041440</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>0.204</v>
+        <v>0.819</v>
       </c>
       <c r="E64" s="0" t="n">
         <f aca="false">B64 * D64</f>
-        <v>0.204</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="2" t="s">
+        <v>8.19</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C65" s="3"/>
+      <c r="B65" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C65" s="5" t="n">
+        <v>671990</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <f aca="false">B65 * D65</f>
+        <v>3.2</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="8" t="s">
+      <c r="A66" s="0" t="s">
         <v>68</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C66" s="7" t="n">
-        <v>3041440</v>
+        <v>1</v>
+      </c>
+      <c r="C66" s="5" t="n">
+        <v>1577768</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>0.819</v>
+        <v>2</v>
       </c>
       <c r="E66" s="0" t="n">
         <f aca="false">B66 * D66</f>
-        <v>8.19</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>69</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C67" s="7" t="n">
-        <v>671990</v>
+        <v>1</v>
+      </c>
+      <c r="C67" s="3" t="n">
+        <v>149056</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>1.6</v>
+        <v>13.46</v>
       </c>
       <c r="E67" s="0" t="n">
         <f aca="false">B67 * D67</f>
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13.46</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>70</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C68" s="7" t="n">
-        <v>1577768</v>
-      </c>
+      <c r="C68" s="3"/>
       <c r="D68" s="0" t="n">
         <v>2</v>
       </c>
@@ -1507,56 +1485,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C70" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B69" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C69" s="3" t="n">
-        <v>149056</v>
-      </c>
-      <c r="D69" s="0" t="n">
-        <v>13.46</v>
-      </c>
-      <c r="E69" s="0" t="n">
-        <f aca="false">B69 * D69</f>
-        <v>13.46</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="E70" s="4" t="n">
+        <f aca="false">SUM(E3:E69)</f>
+        <v>98.6645</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C71" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B70" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C70" s="3"/>
-      <c r="D70" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E70" s="0" t="n">
-        <f aca="false">B70 * D70</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C72" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="E72" s="9" t="n">
-        <f aca="false">SUM(E3:E71)</f>
-        <v>100.4745</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C73" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E73" s="9" t="n">
-        <f aca="false">E72 * 1.21</f>
-        <v>121.574145</v>
+      <c r="E71" s="4" t="n">
+        <f aca="false">E70 * 1.21</f>
+        <v>119.384045</v>
       </c>
     </row>
   </sheetData>

</xml_diff>